<commit_message>
corrections to final xlsx spreadsheet date solutions
</commit_message>
<xml_diff>
--- a/case_study/roster_summer_final.xlsx
+++ b/case_study/roster_summer_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmallett\OneDrive - The Council of State Governments\GitProjects\va_casestudy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg-my.sharepoint.com/personal/jmallett_csg_org/Documents/GitProjects/va_casestudy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67DA349F-5541-47B4-A325-BE8ED9DAF5B7}"/>
   <bookViews>
-    <workbookView xWindow="12705" yWindow="0" windowWidth="24000" windowHeight="21000" activeTab="6" xr2:uid="{49CF00D1-68CA-4DA7-9F84-7A2BC145D750}"/>
+    <workbookView xWindow="-21720" yWindow="765" windowWidth="20955" windowHeight="14265" activeTab="4" xr2:uid="{49CF00D1-68CA-4DA7-9F84-7A2BC145D750}"/>
   </bookViews>
   <sheets>
     <sheet name="roster" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,13 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
-    <pivotCache cacheId="2" r:id="rId9"/>
-    <pivotCache cacheId="3" r:id="rId10"/>
-    <pivotCache cacheId="4" r:id="rId11"/>
-    <pivotCache cacheId="5" r:id="rId12"/>
-    <pivotCache cacheId="18" r:id="rId13"/>
-    <pivotCache cacheId="33" r:id="rId14"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId10"/>
+    <pivotCache cacheId="3" r:id="rId11"/>
+    <pivotCache cacheId="4" r:id="rId12"/>
+    <pivotCache cacheId="5" r:id="rId13"/>
+    <pivotCache cacheId="6" r:id="rId14"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1090,7 +1090,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1108,7 +1108,6 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1154,13 +1153,30 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <fill>
@@ -1224,177 +1240,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <fill>
@@ -3172,7 +3017,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Recidivism Rate 2021-2022</a:t>
+              <a:t>Recidivism Rate 2017-2018</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7139,7 +6984,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7315200" y="9205912"/>
+              <a:off x="7334250" y="9205912"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -9597,7 +9442,259 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BE235AC-8D6C-4094-B02A-08825CA16888}" name="PivotTable2" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1837024C-55B8-4E16-ACBD-6396B821F302}" name="PivotTable8" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A11:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="5"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="15">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of programs" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4EA5A56-04A3-4340-8CB2-F1B0DEAAB37C}" name="PivotTable20" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Clients Served" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BE235AC-8D6C-4094-B02A-08825CA16888}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField numFmtId="14" showAll="0">
@@ -9739,7 +9836,7 @@
     <dataField name="Count of Years (dt)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="8">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -9748,7 +9845,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -9781,88 +9878,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4EA5A56-04A3-4340-8CB2-F1B0DEAAB37C}" name="PivotTable20" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Clients Served" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="G3:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField showAll="0"/>
@@ -9939,7 +9956,7 @@
     <dataField name="Count of prg" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="37">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -9948,7 +9965,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -9957,7 +9974,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="1">
@@ -9990,8 +10007,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF987B5F-D31F-42B0-B08A-18DFC95CC24D}" name="PivotTable10" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF987B5F-D31F-42B0-B08A-18DFC95CC24D}" name="PivotTable10" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D12:D13" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -10021,8 +10038,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64C769B9-9264-4FB6-BE0D-1932A5224F36}" name="PivotTable9" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64C769B9-9264-4FB6-BE0D-1932A5224F36}" name="PivotTable9" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="D3:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -10070,7 +10087,7 @@
     <dataField name="Count of ret" fld="4" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="27">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -10079,7 +10096,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -10088,7 +10105,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -10139,180 +10156,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1837024C-55B8-4E16-ACBD-6396B821F302}" name="PivotTable8" cacheId="33" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A11:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="5"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="11"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="12"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="15">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of programs" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="23">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="25">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="26">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69DFE558-44F1-4255-85E0-5603F9A3D9C1}" name="PivotTable15" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Programs">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69DFE558-44F1-4255-85E0-5603F9A3D9C1}" name="PivotTable15" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Programs">
   <location ref="D3:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField showAll="0"/>
@@ -10400,7 +10245,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E0959C41-F0CD-4094-B6C2-07B7656F42CB}" name="PivotTable12" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E0959C41-F0CD-4094-B6C2-07B7656F42CB}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -10542,7 +10387,7 @@
     </dataField>
   </dataFields>
   <formats count="3">
-    <format dxfId="33">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -10554,7 +10399,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -10566,7 +10411,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="0">
       <pivotArea dataOnly="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -10589,7 +10434,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C7E8ECE4-0EBA-48C7-B8A4-0F72290F0001}" name="PivotTable16" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C7E8ECE4-0EBA-48C7-B8A4-0F72290F0001}" name="PivotTable16" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A4" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -10618,7 +10463,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C531E27B-71EA-462D-8308-9C201C8A2341}" name="PivotTable19" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C531E27B-71EA-462D-8308-9C201C8A2341}" name="PivotTable19" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:C4" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" includeNewItemsInFilter="1">
@@ -10669,7 +10514,7 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9C812EC4-1D21-4A20-AACC-3D8067BDB6E7}" name="client_names"/>
     <tableColumn id="2" xr3:uid="{32DFF5D8-1553-4D48-B733-5DE20CC2AE51}" name="age"/>
-    <tableColumn id="3" xr3:uid="{4B3AA37A-B124-4862-925F-7F1A03806C4E}" name="dt" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{4B3AA37A-B124-4862-925F-7F1A03806C4E}" name="dt" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{71582D88-5DAB-4152-AE0B-5CEFB5FAB47E}" name="programs"/>
     <tableColumn id="5" xr3:uid="{BCDEF0D6-673B-4849-B3E5-B378327051C7}" name="ret"/>
   </tableColumns>
@@ -12681,7 +12526,7 @@
       <c r="D4" s="5">
         <v>-1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -12695,7 +12540,7 @@
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5">
         <v>34</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -12709,7 +12554,7 @@
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6">
         <v>18</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -12723,7 +12568,7 @@
       <c r="D7" s="5">
         <v>2</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -12737,7 +12582,7 @@
       <c r="D8" s="5">
         <v>11</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -12751,7 +12596,7 @@
       <c r="D9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9">
         <v>55</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -12793,7 +12638,7 @@
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12">
         <v>8</v>
       </c>
       <c r="D12" t="s">
@@ -12810,10 +12655,10 @@
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13">
         <v>3</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13">
         <v>28.709090909090911</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -12827,7 +12672,7 @@
       <c r="A14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14">
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -12841,7 +12686,7 @@
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15">
         <v>7</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -12855,7 +12700,7 @@
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16">
         <v>2</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -12869,7 +12714,7 @@
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17">
         <v>6</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -12883,7 +12728,7 @@
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18">
         <v>2</v>
       </c>
     </row>
@@ -12891,7 +12736,7 @@
       <c r="A19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19">
         <v>1</v>
       </c>
     </row>
@@ -12899,7 +12744,7 @@
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20">
         <v>4</v>
       </c>
     </row>
@@ -12907,7 +12752,7 @@
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21">
         <v>3</v>
       </c>
     </row>
@@ -12915,7 +12760,7 @@
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22">
         <v>2</v>
       </c>
     </row>
@@ -12923,7 +12768,7 @@
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23">
         <v>3</v>
       </c>
     </row>
@@ -12931,7 +12776,7 @@
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24">
         <v>4</v>
       </c>
     </row>
@@ -12939,7 +12784,7 @@
       <c r="A25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25">
         <v>9</v>
       </c>
     </row>
@@ -12947,7 +12792,7 @@
       <c r="A26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26">
         <v>55</v>
       </c>
     </row>
@@ -12963,7 +12808,7 @@
       <c r="A30" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30">
         <v>1</v>
       </c>
     </row>
@@ -12971,7 +12816,7 @@
       <c r="A31" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31">
         <v>1</v>
       </c>
     </row>
@@ -12979,7 +12824,7 @@
       <c r="A32" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32">
         <v>24</v>
       </c>
     </row>
@@ -12987,7 +12832,7 @@
       <c r="A33" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33">
         <v>29</v>
       </c>
     </row>
@@ -12995,7 +12840,7 @@
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34">
         <v>55</v>
       </c>
     </row>
@@ -13009,8 +12854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A311EE96-515E-4E71-AE25-43A4EF9BE97D}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13725,7 +13570,7 @@
         <v>41</v>
       </c>
       <c r="C31" s="1">
-        <v>35664</v>
+        <v>42969</v>
       </c>
       <c r="D31" t="s">
         <v>19</v>
@@ -14116,7 +13961,7 @@
         <v>24</v>
       </c>
       <c r="C48" s="1">
-        <v>39238</v>
+        <v>42891</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -14453,8 +14298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA88D4E6-102F-4EC2-B3DB-C67C3776A97B}">
   <dimension ref="A2:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15100,7 +14945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E585C765-9993-4BFA-90B9-04FA964DBB4D}">
   <dimension ref="A3:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated session 3 with weights by year
</commit_message>
<xml_diff>
--- a/case_study/roster_summer_final.xlsx
+++ b/case_study/roster_summer_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg-my.sharepoint.com/personal/jmallett_csg_org/Documents/GitProjects/va_data/case_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E26F8D6-CB84-451D-8820-A46A13A3E941}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2A425F8-62F2-48DC-98B5-E5E826BFF97B}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="713" activeTab="7" xr2:uid="{49CF00D1-68CA-4DA7-9F84-7A2BC145D750}"/>
   </bookViews>
@@ -29,12 +29,12 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="7" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
     <pivotCache cacheId="2" r:id="rId11"/>
-    <pivotCache cacheId="4" r:id="rId12"/>
-    <pivotCache cacheId="5" r:id="rId13"/>
-    <pivotCache cacheId="6" r:id="rId14"/>
-    <pivotCache cacheId="13" r:id="rId15"/>
+    <pivotCache cacheId="3" r:id="rId12"/>
+    <pivotCache cacheId="4" r:id="rId13"/>
+    <pivotCache cacheId="5" r:id="rId14"/>
+    <pivotCache cacheId="7" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="192">
   <si>
     <t>client_names</t>
   </si>
@@ -612,6 +612,24 @@
   <si>
     <t>ret rate (2018)</t>
   </si>
+  <si>
+    <t>weights (2017)</t>
+  </si>
+  <si>
+    <t>weights (2018)</t>
+  </si>
+  <si>
+    <t>Weighted Average 10 programs (2017)</t>
+  </si>
+  <si>
+    <t>Weighted Average 10 programs (2018)</t>
+  </si>
+  <si>
+    <t>Weighted Average 5 programs (2017)</t>
+  </si>
+  <si>
+    <t>Weighted Average 5 programs (2018)</t>
+  </si>
 </sst>
 </file>
 
@@ -1100,7 +1118,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1118,6 +1136,7 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1163,7 +1182,13 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="38">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1305,26 +1330,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -1341,13 +1346,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -11222,111 +11220,24 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64C769B9-9264-4FB6-BE0D-1932A5224F36}" name="PivotTable9" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="D3:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF987B5F-D31F-42B0-B08A-18DFC95CC24D}" name="PivotTable10" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D12:D13" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="6">
-        <item x="4"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
   </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <rowItems count="1">
+    <i/>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of ret" fld="4" subtotal="count" baseField="4" baseItem="0"/>
+    <dataField name="Average of age" fld="1" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="3">
-    <format dxfId="31">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="30">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="29">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -11427,882 +11338,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1837024C-55B8-4E16-ACBD-6396B821F302}" name="PivotTable8" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A11:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="15">
-        <item x="0"/>
-        <item x="5"/>
-        <item x="13"/>
-        <item x="4"/>
-        <item x="11"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="12"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="3"/>
-        <item x="10"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="15">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of programs" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="4">
-    <format dxfId="35">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="34">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="33">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="10"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="32">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="4">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="1" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BE235AC-8D6C-4094-B02A-08825CA16888}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField numFmtId="14" showAll="0">
-      <items count="48">
-        <item x="28"/>
-        <item x="43"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="40"/>
-        <item x="7"/>
-        <item x="27"/>
-        <item x="15"/>
-        <item x="24"/>
-        <item x="6"/>
-        <item x="44"/>
-        <item x="36"/>
-        <item x="41"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="33"/>
-        <item x="0"/>
-        <item x="45"/>
-        <item x="34"/>
-        <item x="38"/>
-        <item x="30"/>
-        <item x="17"/>
-        <item x="25"/>
-        <item x="22"/>
-        <item x="14"/>
-        <item x="19"/>
-        <item x="5"/>
-        <item x="31"/>
-        <item x="39"/>
-        <item x="18"/>
-        <item x="42"/>
-        <item x="1"/>
-        <item x="46"/>
-        <item x="35"/>
-        <item x="29"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="26"/>
-        <item x="16"/>
-        <item x="3"/>
-        <item x="13"/>
-        <item x="23"/>
-        <item x="37"/>
-        <item x="12"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="32"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="15">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="25">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item sd="0" x="14"/>
-        <item sd="0" x="15"/>
-        <item sd="0" x="16"/>
-        <item sd="0" x="17"/>
-        <item sd="0" x="18"/>
-        <item sd="0" x="19"/>
-        <item sd="0" x="20"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="22"/>
-        <item sd="0" x="23"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Years (dt)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="37">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="4" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="G3:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="14">
-        <item x="6"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="10"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="14">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of prg" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="40">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="39">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="38">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF987B5F-D31F-42B0-B08A-18DFC95CC24D}" name="PivotTable10" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D12:D13" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Average of age" fld="1" subtotal="average" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69DFE558-44F1-4255-85E0-5603F9A3D9C1}" name="PivotTable15" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Programs">
-  <location ref="D3:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="11">
-        <item x="5"/>
-        <item x="9"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="staff count" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E0959C41-F0CD-4094-B6C2-07B7656F42CB}" name="PivotTable12" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="12">
-        <item x="0"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="8"/>
-        <item m="1" x="10"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="3"/>
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="31">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of ret" fld="4" subtotal="count" baseField="3" baseItem="0" numFmtId="10">
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
-          <x14:dataField pivotShowAs="percentOfParentRow"/>
-        </ext>
-      </extLst>
-    </dataField>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="22">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="3" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="23">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="3" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="24">
-      <pivotArea dataOnly="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4EA5A56-04A3-4340-8CB2-F1B0DEAAB37C}" name="PivotTable20" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Clients Served" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E52A3FAF-5430-4F6E-B896-232940CED406}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E52A3FAF-5430-4F6E-B896-232940CED406}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -12461,7 +11498,7 @@
     </dataField>
   </dataFields>
   <formats count="20">
-    <format dxfId="19">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12474,7 +11511,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12486,7 +11523,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="19">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12499,7 +11536,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12511,7 +11548,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12524,7 +11561,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12536,7 +11573,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="15">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12549,7 +11586,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12561,7 +11598,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12574,7 +11611,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12586,7 +11623,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12599,7 +11636,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12611,7 +11648,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="9">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12624,7 +11661,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12636,7 +11673,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12649,7 +11686,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12661,7 +11698,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12674,7 +11711,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12686,7 +11723,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1" selected="0">
@@ -12699,7 +11736,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="3" count="1" selected="0">
@@ -12724,13 +11761,1072 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64C769B9-9264-4FB6-BE0D-1932A5224F36}" name="PivotTable9" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="D3:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ret" fld="4" subtotal="count" baseField="4" baseItem="0"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="28">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1837024C-55B8-4E16-ACBD-6396B821F302}" name="PivotTable8" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A11:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="15">
+        <item x="0"/>
+        <item x="5"/>
+        <item x="13"/>
+        <item x="4"/>
+        <item x="11"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="3"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="15">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of programs" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="4">
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BE235AC-8D6C-4094-B02A-08825CA16888}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField numFmtId="14" showAll="0">
+      <items count="48">
+        <item x="28"/>
+        <item x="43"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="40"/>
+        <item x="7"/>
+        <item x="27"/>
+        <item x="15"/>
+        <item x="24"/>
+        <item x="6"/>
+        <item x="44"/>
+        <item x="36"/>
+        <item x="41"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="33"/>
+        <item x="0"/>
+        <item x="45"/>
+        <item x="34"/>
+        <item x="38"/>
+        <item x="30"/>
+        <item x="17"/>
+        <item x="25"/>
+        <item x="22"/>
+        <item x="14"/>
+        <item x="19"/>
+        <item x="5"/>
+        <item x="31"/>
+        <item x="39"/>
+        <item x="18"/>
+        <item x="42"/>
+        <item x="1"/>
+        <item x="46"/>
+        <item x="35"/>
+        <item x="29"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="26"/>
+        <item x="16"/>
+        <item x="3"/>
+        <item x="13"/>
+        <item x="23"/>
+        <item x="37"/>
+        <item x="12"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="32"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="15">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="25">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Years (dt)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="34">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="3" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="4" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="G3:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="14">
+        <item x="6"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of prg" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="36">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="35">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{69DFE558-44F1-4255-85E0-5603F9A3D9C1}" name="PivotTable15" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Programs">
+  <location ref="D3:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="11">
+        <item x="5"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="staff count" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E0959C41-F0CD-4094-B6C2-07B7656F42CB}" name="PivotTable12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item m="1" x="10"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ret" fld="4" subtotal="count" baseField="3" baseItem="0" numFmtId="10">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
+          <x14:dataField pivotShowAs="percentOfParentRow"/>
+        </ext>
+      </extLst>
+    </dataField>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="24">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="23">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4EA5A56-04A3-4340-8CB2-F1B0DEAAB37C}" name="PivotTable20" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Clients Served" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{015DAE7A-17B5-408F-80AF-68680B1C977B}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A38:D50" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Clients Served" fld="3" subtotal="count" baseField="3" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F061CD81-9E88-4568-85F2-99F0627C4384}" name="Table1" displayName="Table1" ref="A1:E51" totalsRowShown="0">
   <autoFilter ref="A1:E51" xr:uid="{F061CD81-9E88-4568-85F2-99F0627C4384}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9C812EC4-1D21-4A20-AACC-3D8067BDB6E7}" name="client_names"/>
     <tableColumn id="2" xr3:uid="{32DFF5D8-1553-4D48-B733-5DE20CC2AE51}" name="age"/>
-    <tableColumn id="3" xr3:uid="{4B3AA37A-B124-4862-925F-7F1A03806C4E}" name="dt" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{4B3AA37A-B124-4862-925F-7F1A03806C4E}" name="dt" dataDxfId="25"/>
     <tableColumn id="4" xr3:uid="{71582D88-5DAB-4152-AE0B-5CEFB5FAB47E}" name="programs"/>
     <tableColumn id="5" xr3:uid="{BCDEF0D6-673B-4849-B3E5-B378327051C7}" name="ret"/>
   </tableColumns>
@@ -12755,10 +12851,10 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5274F79A-C733-4538-959B-108EBE859F16}" name="client_names"/>
     <tableColumn id="2" xr3:uid="{AA1CC566-36D8-43BE-AC51-E96AC3BACE89}" name="age"/>
-    <tableColumn id="3" xr3:uid="{B61A1EC3-7C5B-489F-B582-8AA65FE7282D}" name="dt" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{B61A1EC3-7C5B-489F-B582-8AA65FE7282D}" name="dt" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{826EAD0A-7A59-4B30-A33B-9715EBF15597}" name="programs"/>
     <tableColumn id="5" xr3:uid="{D1EED26A-D043-437E-BE00-FA80072D5269}" name="ret"/>
-    <tableColumn id="6" xr3:uid="{F60D58A3-D0E9-4262-B243-2DCA694F8735}" name="YEAR(dt)" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{F60D58A3-D0E9-4262-B243-2DCA694F8735}" name="YEAR(dt)" dataDxfId="0">
       <calculatedColumnFormula>YEAR(Table14[[#This Row],[dt]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -17078,7 +17174,7 @@
   <dimension ref="A3:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17249,17 +17345,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625428BA-622F-4059-9BDC-96508CD558EE}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="13.140625" bestFit="1" customWidth="1"/>
@@ -18779,6 +18875,12 @@
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="U38" t="s">
         <v>53</v>
       </c>
@@ -18800,6 +18902,30 @@
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>2017</v>
+      </c>
+      <c r="C39">
+        <v>2018</v>
+      </c>
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" t="s">
+        <v>187</v>
+      </c>
+      <c r="H39" t="s">
+        <v>188</v>
+      </c>
+      <c r="L39" t="s">
+        <v>190</v>
+      </c>
       <c r="U39" t="s">
         <v>54</v>
       </c>
@@ -18821,6 +18947,34 @@
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="9">
+        <v>3</v>
+      </c>
+      <c r="C40" s="9">
+        <v>4</v>
+      </c>
+      <c r="D40" s="9">
+        <v>7</v>
+      </c>
+      <c r="E40">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","am","YEAR(dt)",2017)*I4</f>
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","am","YEAR(dt)",2018)*J4</f>
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <f>SUM(E40:E49)/GETPIVOTDATA("programs",$A$38,"YEAR(dt)",2017)</f>
+        <v>0.4</v>
+      </c>
+      <c r="L40">
+        <f>SUM(E40,E43,E44,E46,E49)/SUM(B40,B43,B44,B46,B49)</f>
+        <v>0.46666666666666667</v>
+      </c>
       <c r="U40" t="s">
         <v>55</v>
       </c>
@@ -18842,6 +18996,32 @@
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="9">
+        <v>2</v>
+      </c>
+      <c r="C41" s="9">
+        <v>2</v>
+      </c>
+      <c r="D41" s="9">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","bcs","YEAR(dt)",2017)*I5</f>
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","bcs","YEAR(dt)",2018)*J5</f>
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>189</v>
+      </c>
+      <c r="L41" t="s">
+        <v>191</v>
+      </c>
       <c r="U41" t="s">
         <v>56</v>
       </c>
@@ -18863,6 +19043,34 @@
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="9">
+        <v>3</v>
+      </c>
+      <c r="C42" s="9">
+        <v>5</v>
+      </c>
+      <c r="D42" s="9">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","brave","YEAR(dt)",2017)*I6</f>
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","brave","YEAR(dt)",2018)*J6</f>
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <f>SUM(F40:F49)/GETPIVOTDATA("programs",$A$38,"YEAR(dt)",2018)</f>
+        <v>0.36</v>
+      </c>
+      <c r="L42">
+        <f>SUM(F40,F43,F44,F46,F49)/SUM(C40,C43,C44,C46,C49)</f>
+        <v>0.35714285714285715</v>
+      </c>
       <c r="U42" t="s">
         <v>57</v>
       </c>
@@ -18884,6 +19092,26 @@
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="9">
+        <v>3</v>
+      </c>
+      <c r="C43" s="9">
+        <v>3</v>
+      </c>
+      <c r="D43" s="9">
+        <v>6</v>
+      </c>
+      <c r="E43">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","challenge","YEAR(dt)",2017)*I7</f>
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","challenge","YEAR(dt)",2018)*J7</f>
+        <v>1</v>
+      </c>
       <c r="U43" t="s">
         <v>58</v>
       </c>
@@ -18905,6 +19133,26 @@
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="9">
+        <v>2</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","dbt","YEAR(dt)",2017)*I8</f>
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","dbt","YEAR(dt)",2018)*J8</f>
+        <v>0</v>
+      </c>
       <c r="U44" t="s">
         <v>59</v>
       </c>
@@ -18926,6 +19174,26 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9">
+        <v>2</v>
+      </c>
+      <c r="D45" s="9">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","mhsd","YEAR(dt)",2017)*I9</f>
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","mhsd","YEAR(dt)",2018)*J9</f>
+        <v>1</v>
+      </c>
       <c r="U45" t="s">
         <v>61</v>
       </c>
@@ -18947,6 +19215,26 @@
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="9">
+        <v>2</v>
+      </c>
+      <c r="C46" s="9">
+        <v>2</v>
+      </c>
+      <c r="D46" s="9">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","rdap","YEAR(dt)",2017)*I10</f>
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","rdap","YEAR(dt)",2018)*J10</f>
+        <v>1</v>
+      </c>
       <c r="U46" t="s">
         <v>62</v>
       </c>
@@ -18968,6 +19256,24 @@
       </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="9">
+        <v>3</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","resolve","YEAR(dt)",2017)*I11</f>
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","resolve","YEAR(dt)",2018)*J11</f>
+        <v>0</v>
+      </c>
       <c r="U47" t="s">
         <v>63</v>
       </c>
@@ -18989,6 +19295,26 @@
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+      <c r="C48" s="9">
+        <v>2</v>
+      </c>
+      <c r="D48" s="9">
+        <v>3</v>
+      </c>
+      <c r="E48">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","sotrt","YEAR(dt)",2017)*I12</f>
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","sotrt","YEAR(dt)",2018)*J12</f>
+        <v>1</v>
+      </c>
       <c r="U48" t="s">
         <v>64</v>
       </c>
@@ -19009,7 +19335,27 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="49" spans="21:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="9">
+        <v>5</v>
+      </c>
+      <c r="C49" s="9">
+        <v>4</v>
+      </c>
+      <c r="D49" s="9">
+        <v>9</v>
+      </c>
+      <c r="E49">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","stages","YEAR(dt)",2017)*I13</f>
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <f>GETPIVOTDATA("programs",$A$38,"programs","stages","YEAR(dt)",2018)*J13</f>
+        <v>2</v>
+      </c>
       <c r="U49" t="s">
         <v>65</v>
       </c>
@@ -19030,7 +19376,19 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="50" spans="21:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" s="9">
+        <v>25</v>
+      </c>
+      <c r="C50" s="9">
+        <v>25</v>
+      </c>
+      <c r="D50" s="9">
+        <v>50</v>
+      </c>
       <c r="U50" t="s">
         <v>66</v>
       </c>
@@ -19051,7 +19409,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="51" spans="21:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="U51" t="s">
         <v>67</v>
       </c>
@@ -19074,9 +19432,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected missing data in solution
</commit_message>
<xml_diff>
--- a/case_study/roster_summer_final.xlsx
+++ b/case_study/roster_summer_final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg-my.sharepoint.com/personal/jmallett_csg_org/Documents/GitProjects/va_data/case_study/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg-my.sharepoint.com/personal/jmallett_csg_org/Documents/GitProjects/va_casestudy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2A425F8-62F2-48DC-98B5-E5E826BFF97B}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2193EA2D-0076-439D-8452-D82E25F8B4FB}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="713" activeTab="7" xr2:uid="{49CF00D1-68CA-4DA7-9F84-7A2BC145D750}"/>
   </bookViews>
@@ -34,7 +34,7 @@
     <pivotCache cacheId="3" r:id="rId12"/>
     <pivotCache cacheId="4" r:id="rId13"/>
     <pivotCache cacheId="5" r:id="rId14"/>
-    <pivotCache cacheId="7" r:id="rId15"/>
+    <pivotCache cacheId="6" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1118,7 +1118,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1136,7 +1136,6 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3982,9 +3981,6 @@
                 <c:pt idx="6">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="8">
                   <c:v>0.5</c:v>
                 </c:pt>
@@ -11220,24 +11216,122 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF987B5F-D31F-42B0-B08A-18DFC95CC24D}" name="PivotTable10" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D12:D13" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="G3:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="14">
+        <item x="6"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowItems count="1">
-    <i/>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of age" fld="1" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Count of prg" fld="1" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <formats count="3">
+    <format dxfId="28">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="27">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="26">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -11339,7 +11433,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E52A3FAF-5430-4F6E-B896-232940CED406}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E52A3FAF-5430-4F6E-B896-232940CED406}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D35" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -11762,6 +11856,37 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF987B5F-D31F-42B0-B08A-18DFC95CC24D}" name="PivotTable10" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D12:D13" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of age" fld="1" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64C769B9-9264-4FB6-BE0D-1932A5224F36}" name="PivotTable9" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="D3:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
@@ -11810,7 +11935,7 @@
     <dataField name="Count of ret" fld="4" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="28">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -11819,7 +11944,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -11828,7 +11953,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -11879,7 +12004,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1837024C-55B8-4E16-ACBD-6396B821F302}" name="PivotTable8" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A11:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
@@ -11964,7 +12089,7 @@
     <dataField name="Count of programs" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="32">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -11973,7 +12098,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -11982,7 +12107,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -11991,7 +12116,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -12051,7 +12176,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BE235AC-8D6C-4094-B02A-08825CA16888}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -12194,7 +12319,7 @@
     <dataField name="Count of Years (dt)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="34">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -12203,7 +12328,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -12215,135 +12340,6 @@
   </formats>
   <chartFormats count="1">
     <chartFormat chart="4" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="G3:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="14">
-        <item x="6"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="10"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="12"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="14">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of prg" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="3">
-    <format dxfId="37">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="35">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -12723,7 +12719,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{015DAE7A-17B5-408F-80AF-68680B1C977B}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{015DAE7A-17B5-408F-80AF-68680B1C977B}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A38:D50" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -17174,7 +17170,7 @@
   <dimension ref="A3:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17345,15 +17341,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625428BA-622F-4059-9BDC-96508CD558EE}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -17805,10 +17801,6 @@
         <f>GETPIVOTDATA("ret",$A$3,"programs","resolve","ret",1,"YEAR(dt)",2017)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J11">
-        <f>GETPIVOTDATA("ret",$A$3,"programs","resolve","ret",1,"YEAR(dt)",2018)</f>
-        <v>0</v>
-      </c>
       <c r="U11" t="s">
         <v>20</v>
       </c>
@@ -18411,10 +18403,6 @@
         <f>GETPIVOTDATA("ret",$A$3,"programs","resolve","ret",1,"YEAR(dt)",2017)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J24">
-        <f>GETPIVOTDATA("ret",$A$3,"programs","resolve","ret",1,"YEAR(dt)",2018)</f>
-        <v>0</v>
-      </c>
       <c r="U24" t="s">
         <v>36</v>
       </c>
@@ -18950,13 +18938,13 @@
       <c r="A40" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40">
         <v>3</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40">
         <v>4</v>
       </c>
-      <c r="D40" s="9">
+      <c r="D40">
         <v>7</v>
       </c>
       <c r="E40">
@@ -18999,13 +18987,13 @@
       <c r="A41" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41">
         <v>2</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41">
         <v>2</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41">
         <v>4</v>
       </c>
       <c r="E41">
@@ -19046,13 +19034,13 @@
       <c r="A42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42">
         <v>3</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42">
         <v>5</v>
       </c>
-      <c r="D42" s="9">
+      <c r="D42">
         <v>8</v>
       </c>
       <c r="E42">
@@ -19095,13 +19083,13 @@
       <c r="A43" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43">
         <v>3</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43">
         <v>3</v>
       </c>
-      <c r="D43" s="9">
+      <c r="D43">
         <v>6</v>
       </c>
       <c r="E43">
@@ -19136,13 +19124,13 @@
       <c r="A44" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44">
         <v>2</v>
       </c>
-      <c r="C44" s="9">
+      <c r="C44">
         <v>1</v>
       </c>
-      <c r="D44" s="9">
+      <c r="D44">
         <v>3</v>
       </c>
       <c r="E44">
@@ -19177,13 +19165,13 @@
       <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45">
         <v>2</v>
       </c>
-      <c r="D45" s="9">
+      <c r="D45">
         <v>3</v>
       </c>
       <c r="E45">
@@ -19218,13 +19206,13 @@
       <c r="A46" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46">
         <v>2</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46">
         <v>2</v>
       </c>
-      <c r="D46" s="9">
+      <c r="D46">
         <v>4</v>
       </c>
       <c r="E46">
@@ -19259,21 +19247,16 @@
       <c r="A47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47">
         <v>3</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9">
+      <c r="D47">
         <v>3</v>
       </c>
       <c r="E47">
         <f>GETPIVOTDATA("programs",$A$38,"programs","resolve","YEAR(dt)",2017)*I11</f>
         <v>1</v>
       </c>
-      <c r="F47">
-        <f>GETPIVOTDATA("programs",$A$38,"programs","resolve","YEAR(dt)",2018)*J11</f>
-        <v>0</v>
-      </c>
       <c r="U47" t="s">
         <v>63</v>
       </c>
@@ -19298,13 +19281,13 @@
       <c r="A48" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48">
         <v>1</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48">
         <v>2</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D48">
         <v>3</v>
       </c>
       <c r="E48">
@@ -19339,13 +19322,13 @@
       <c r="A49" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49">
         <v>5</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49">
         <v>4</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D49">
         <v>9</v>
       </c>
       <c r="E49">
@@ -19380,13 +19363,13 @@
       <c r="A50" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50">
         <v>25</v>
       </c>
-      <c r="C50" s="9">
+      <c r="C50">
         <v>25</v>
       </c>
-      <c r="D50" s="9">
+      <c r="D50">
         <v>50</v>
       </c>
       <c r="U50" t="s">

</xml_diff>

<commit_message>
updated with a descriptions of sheets tab
</commit_message>
<xml_diff>
--- a/case_study/roster_summer_final.xlsx
+++ b/case_study/roster_summer_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg-my.sharepoint.com/personal/jmallett_csg_org/Documents/GitProjects/va_casestudy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgorg-my.sharepoint.com/personal/jmallett_csg_org/Documents/GitProjects/va_data/case_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2193EA2D-0076-439D-8452-D82E25F8B4FB}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{D021C4DC-C3A6-4C70-8087-F8BD10030BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0211746-24AE-4DF2-B2EA-DDC66C76F196}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="713" activeTab="7" xr2:uid="{49CF00D1-68CA-4DA7-9F84-7A2BC145D750}"/>
+    <workbookView xWindow="735" yWindow="0" windowWidth="32025" windowHeight="21000" tabRatio="821" activeTab="8" xr2:uid="{49CF00D1-68CA-4DA7-9F84-7A2BC145D750}"/>
   </bookViews>
   <sheets>
     <sheet name="roster" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Session2 Task1" sheetId="8" r:id="rId6"/>
     <sheet name="Session2 Task2" sheetId="7" r:id="rId7"/>
     <sheet name="Session3" sheetId="10" r:id="rId8"/>
+    <sheet name="Descriptions" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">roster!$B$1</definedName>
@@ -28,13 +29,13 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
-    <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="2" r:id="rId11"/>
-    <pivotCache cacheId="3" r:id="rId12"/>
-    <pivotCache cacheId="4" r:id="rId13"/>
-    <pivotCache cacheId="5" r:id="rId14"/>
-    <pivotCache cacheId="6" r:id="rId15"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="2" r:id="rId12"/>
+    <pivotCache cacheId="3" r:id="rId13"/>
+    <pivotCache cacheId="4" r:id="rId14"/>
+    <pivotCache cacheId="5" r:id="rId15"/>
+    <pivotCache cacheId="6" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="213">
   <si>
     <t>client_names</t>
   </si>
@@ -629,13 +630,76 @@
   </si>
   <si>
     <t>Weighted Average 5 programs (2018)</t>
+  </si>
+  <si>
+    <t>SHEET</t>
+  </si>
+  <si>
+    <t>SESSION</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>roster</t>
+  </si>
+  <si>
+    <t>Lab Task1 Explore</t>
+  </si>
+  <si>
+    <t>Lab Task1 Clean</t>
+  </si>
+  <si>
+    <t>Lab Task23</t>
+  </si>
+  <si>
+    <t>Session2 Task1</t>
+  </si>
+  <si>
+    <t>Session2 Task2</t>
+  </si>
+  <si>
+    <t>Session3</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>DESCRIPTION OF CONTENTS</t>
+  </si>
+  <si>
+    <t>raw roster dataset</t>
+  </si>
+  <si>
+    <t>raw staff dataset</t>
+  </si>
+  <si>
+    <t>breakouts of all dataset variables, plots of all variables</t>
+  </si>
+  <si>
+    <t>fully cleaned roster and staff datasets</t>
+  </si>
+  <si>
+    <t>table of recidivism rates and staffing for each program, and plot of recidivism rates by program</t>
+  </si>
+  <si>
+    <t>average recidivism rates pooled years (overall programs, and over just 5 CWC programs) UNWEIGHTED</t>
+  </si>
+  <si>
+    <t>average recidivism rates pooled years (overall programs, and over just 5 CWC programs) WEIGHTED</t>
+  </si>
+  <si>
+    <t>program recidivism rates by year, average recidivism rates across all programs by year, and over just 5 CWC programs by year WEIGHTED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -766,6 +830,23 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1118,7 +1199,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -1136,6 +1217,8 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3191,7 +3274,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Recidivism Rate 2017-2018</a:t>
+              <a:t>Recidivism Rate </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Program Years 2017-2018</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3739,7 +3831,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Recidivism Rate 2017-2018</a:t>
+              <a:t>Recidivism Rate </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Program Years 2017-2018</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11216,71 +11317,136 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="G3:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField showAll="0"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BE235AC-8D6C-4094-B02A-08825CA16888}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField numFmtId="14" showAll="0">
+      <items count="48">
+        <item x="28"/>
+        <item x="43"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="40"/>
+        <item x="7"/>
+        <item x="27"/>
+        <item x="15"/>
+        <item x="24"/>
+        <item x="6"/>
+        <item x="44"/>
+        <item x="36"/>
+        <item x="41"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="33"/>
+        <item x="0"/>
+        <item x="45"/>
+        <item x="34"/>
+        <item x="38"/>
+        <item x="30"/>
+        <item x="17"/>
+        <item x="25"/>
+        <item x="22"/>
+        <item x="14"/>
+        <item x="19"/>
+        <item x="5"/>
+        <item x="31"/>
+        <item x="39"/>
+        <item x="18"/>
+        <item x="42"/>
+        <item x="1"/>
+        <item x="46"/>
+        <item x="35"/>
+        <item x="29"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="26"/>
+        <item x="16"/>
+        <item x="3"/>
+        <item x="13"/>
+        <item x="23"/>
+        <item x="37"/>
+        <item x="12"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="32"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="15">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="7">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="14">
-        <item x="6"/>
-        <item x="11"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="10"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="5"/>
-        <item x="9"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="12"/>
+      <items count="25">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
         <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
   <rowFields count="1">
-    <field x="1"/>
+    <field x="3"/>
   </rowFields>
-  <rowItems count="14">
-    <i>
-      <x/>
-    </i>
+  <rowItems count="5">
     <i>
       <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
     </i>
     <i>
       <x v="11"/>
     </i>
     <i>
-      <x v="12"/>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
     </i>
     <i t="grand">
       <x/>
@@ -11290,23 +11456,14 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of prg" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of Years (dt)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="3">
-    <format dxfId="28">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="1" count="1">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
+  <formats count="2">
     <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="8"/>
+          <reference field="3" count="1">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -11314,15 +11471,15 @@
     <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
-          <reference field="1" count="1">
-            <x v="12"/>
+          <reference field="3" count="1">
+            <x v="11"/>
           </reference>
         </references>
       </pivotArea>
     </format>
   </formats>
   <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
+    <chartFormat chart="4" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -11856,6 +12013,135 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{711B3E10-221F-4BDF-B16C-A9E00C5425ED}" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="G3:H17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="14">
+        <item x="6"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="10"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of prg" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="29">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="28">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF987B5F-D31F-42B0-B08A-18DFC95CC24D}" name="PivotTable10" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D12:D13" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="5">
@@ -11886,7 +12172,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{64C769B9-9264-4FB6-BE0D-1932A5224F36}" name="PivotTable9" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="D3:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
@@ -11935,7 +12221,7 @@
     <dataField name="Count of ret" fld="4" subtotal="count" baseField="4" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="31">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -11944,7 +12230,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -11953,7 +12239,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="4" count="1">
@@ -12004,7 +12290,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1837024C-55B8-4E16-ACBD-6396B821F302}" name="PivotTable8" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A11:B26" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
@@ -12089,7 +12375,7 @@
     <dataField name="Count of programs" fld="3" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="35">
+    <format dxfId="37">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -12098,7 +12384,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -12107,7 +12393,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -12116,7 +12402,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="3" count="1">
@@ -12155,191 +12441,6 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="3" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BE235AC-8D6C-4094-B02A-08825CA16888}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="4">
-    <pivotField numFmtId="14" showAll="0">
-      <items count="48">
-        <item x="28"/>
-        <item x="43"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="40"/>
-        <item x="7"/>
-        <item x="27"/>
-        <item x="15"/>
-        <item x="24"/>
-        <item x="6"/>
-        <item x="44"/>
-        <item x="36"/>
-        <item x="41"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="33"/>
-        <item x="0"/>
-        <item x="45"/>
-        <item x="34"/>
-        <item x="38"/>
-        <item x="30"/>
-        <item x="17"/>
-        <item x="25"/>
-        <item x="22"/>
-        <item x="14"/>
-        <item x="19"/>
-        <item x="5"/>
-        <item x="31"/>
-        <item x="39"/>
-        <item x="18"/>
-        <item x="42"/>
-        <item x="1"/>
-        <item x="46"/>
-        <item x="35"/>
-        <item x="29"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="26"/>
-        <item x="16"/>
-        <item x="3"/>
-        <item x="13"/>
-        <item x="23"/>
-        <item x="37"/>
-        <item x="12"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="32"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="15">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="7">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="25">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="8"/>
-        <item sd="0" x="9"/>
-        <item sd="0" x="10"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="13"/>
-        <item sd="0" x="14"/>
-        <item sd="0" x="15"/>
-        <item sd="0" x="16"/>
-        <item sd="0" x="17"/>
-        <item sd="0" x="18"/>
-        <item sd="0" x="19"/>
-        <item sd="0" x="20"/>
-        <item sd="0" x="21"/>
-        <item sd="0" x="22"/>
-        <item sd="0" x="23"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Years (dt)" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="2">
-    <format dxfId="37">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="4" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -13177,7 +13278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1C7B43-D117-4E0E-9A2F-A221698C9E5D}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -15179,7 +15280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A311EE96-515E-4E71-AE25-43A4EF9BE97D}">
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E51"/>
     </sheetView>
   </sheetViews>
@@ -17341,8 +17442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625428BA-622F-4059-9BDC-96508CD558EE}">
   <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19420,4 +19521,151 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB0679F-8322-4CCB-8D88-54B00BFC00C9}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="123.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>